<commit_message>
Added: TC1.5 state Census CSV file with incorrect Column
</commit_message>
<xml_diff>
--- a/src/main/resources/IndiaStateCensusData2.xlsx
+++ b/src/main/resources/IndiaStateCensusData2.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="3660" yWindow="3720" windowWidth="16320" windowHeight="3765"/>
   </bookViews>
   <sheets>
     <sheet name="IndiaStateCensusData2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Population</t>
   </si>
@@ -110,6 +111,9 @@
   </si>
   <si>
     <t>Sikkim</t>
+  </si>
+  <si>
+    <t>State</t>
   </si>
 </sst>
 </file>
@@ -933,11 +937,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>

</xml_diff>